<commit_message>
Merge SFT tables into LON tables
</commit_message>
<xml_diff>
--- a/docs/source/_static/structure/IFDAT-LIST.xlsx
+++ b/docs/source/_static/structure/IFDAT-LIST.xlsx
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ΠΕΡΙΕΧΟΜΕΝΑ'!$A$1:$A$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ΜΠΣ'!$A$1:$F$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'EO'!$A$1:$I$255</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ΕΚΔΟΣΕΙΣ ΜΕΤΟΧΩΝ ΕΟ'!$A$1:$D$341</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ΕΚΔΟΣΕΙΣ ΜΕΤΟΧΩΝ ΕΟ'!$A$1:$D$339</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'ΕΚΔΟΣΕΙΣ ΟΜΟΛΟΓΩΝ ΕΟ'!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -586,7 +586,7 @@
         <is>
           <t>IFDAT
 ΠΙΝΑΚΑΣ ΥΠΟΧΡΕΩΝ ΦΟΡΕΩΝ
-ΗΜΕΡΟΜΗΝΙΑ ΑΝΑΦΟΡΑΣ: 2024-10-29</t>
+ΗΜΕΡΟΜΗΝΙΑ ΑΝΑΦΟΡΑΣ: 2024-11-05</t>
         </is>
       </c>
       <c r="D3" s="1" t="n"/>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B2" s="6" t="inlineStr">
         <is>
-          <t>TGR094282521, BGR000920101000, L213800SHGGWDBFVRPS03</t>
+          <t>TGR094282521, L213800SHGGWDBFVRPS03, BGR000920101000</t>
         </is>
       </c>
       <c r="C2" s="11" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>TGR094036844, L213800BEX8X28DTL5391, BGR000352001000</t>
+          <t>BGR000352001000, L213800BEX8X28DTL5391, TGR094036844</t>
         </is>
       </c>
       <c r="C3" s="13" t="n">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
-          <t>L213800SMPWZVT6GGQZ69, BGR002292401000, TGR094493219</t>
+          <t>BGR002292401000, L213800SMPWZVT6GGQZ69, TGR094493219</t>
         </is>
       </c>
       <c r="C4" s="11" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>L213800C9JGYAXWYTM652, BGR004307701000, TGR099936130</t>
+          <t>BGR004307701000, L213800C9JGYAXWYTM652, TGR099936130</t>
         </is>
       </c>
       <c r="C5" s="13" t="n">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>TGR999081601, BGR006314201000, L213800CF8C4B9AKV1Z96</t>
+          <t>TGR999081601, L213800CF8C4B9AKV1Z96, BGR006314201000</t>
         </is>
       </c>
       <c r="C6" s="11" t="n">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>TGR094304867, BGR001003501000, L213800UWXVWAKFGVLB36</t>
+          <t>L213800UWXVWAKFGVLB36, BGR001003501000, TGR094304867</t>
         </is>
       </c>
       <c r="C7" s="13" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>BGR000942001000, L213800U6WAX3YXMFVH22, TGR094354938</t>
+          <t>L213800U6WAX3YXMFVH22, BGR000942001000, TGR094354938</t>
         </is>
       </c>
       <c r="C8" s="11" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>TGR094325107, L213800YSZHWSCLXXRI37, BGR000832401000</t>
+          <t>BGR000832401000, L213800YSZHWSCLXXRI37, TGR094325107</t>
         </is>
       </c>
       <c r="C9" s="13" t="n">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
-          <t>BGR000918601000, L635400S5G5WWGN6B8T87, TGR094351475</t>
+          <t>TGR094351475, BGR000918601000, L635400S5G5WWGN6B8T87</t>
         </is>
       </c>
       <c r="C10" s="11" t="n">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>L213800XXMES8I6GQVQ47, BGR003581901000, TGR099553209</t>
+          <t>TGR099553209, L213800XXMES8I6GQVQ47, BGR003581901000</t>
         </is>
       </c>
       <c r="C11" s="13" t="n">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>BGR003931601000, TGR099760120, L549300JSLNCWDXJT4U81</t>
+          <t>L549300JSLNCWDXJT4U81, BGR003931601000, TGR099760120</t>
         </is>
       </c>
       <c r="C12" s="11" t="n">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>BGR003882701000, TGR099759863, L213800USGL7Q5UR9M221</t>
+          <t>L213800USGL7Q5UR9M221, BGR003882701000, TGR099759863</t>
         </is>
       </c>
       <c r="C13" s="13" t="n">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
-          <t>L984500EE5E3BA3F08B21, BGR004373001000, TGR999984680</t>
+          <t>BGR004373001000, L984500EE5E3BA3F08B21, TGR999984680</t>
         </is>
       </c>
       <c r="C14" s="11" t="n">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>L213800U7SBKWW79CBG88, TGR099554901, BGR003548801000</t>
+          <t>L213800U7SBKWW79CBG88, BGR003548801000, TGR099554901</t>
         </is>
       </c>
       <c r="C15" s="13" t="n">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="B16" s="6" t="inlineStr">
         <is>
-          <t>TGR998940936, L213800P8QPUPE3SOGX14, BGR006816701000</t>
+          <t>TGR998940936, BGR006816701000, L213800P8QPUPE3SOGX14</t>
         </is>
       </c>
       <c r="C16" s="11" t="n">
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>BGR007175901000, TGR998642355, L2138001MKHE9G2UERJ13</t>
+          <t>L2138001MKHE9G2UERJ13, TGR998642355, BGR007175901000</t>
         </is>
       </c>
       <c r="C17" s="13" t="n">
@@ -1743,7 +1743,7 @@
       </c>
       <c r="B18" s="6" t="inlineStr">
         <is>
-          <t>BGR003546201000, TGR099555020, L549300XDXYOF57JOFT72</t>
+          <t>TGR099555020, BGR003546201000, L549300XDXYOF57JOFT72</t>
         </is>
       </c>
       <c r="C18" s="11" t="n">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B20" s="6" t="inlineStr">
         <is>
-          <t>L213800ESHXNWYJAEMO70, TGR998159392, BGR008234001000</t>
+          <t>BGR008234001000, TGR998159392, L213800ESHXNWYJAEMO70</t>
         </is>
       </c>
       <c r="C20" s="11" t="n">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>L213800QM2ZFRARYU6C87, TGR800397001, BGR120108101000</t>
+          <t>TGR800397001, BGR120108101000, L213800QM2ZFRARYU6C87</t>
         </is>
       </c>
       <c r="C21" s="13" t="n">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="B22" s="6" t="inlineStr">
         <is>
-          <t>L21380099L8WQI3DI3Y74, TGR800398384, BGR120129501000</t>
+          <t>BGR120129501000, TGR800398384, L21380099L8WQI3DI3Y74</t>
         </is>
       </c>
       <c r="C22" s="11" t="n">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>L2138006SQBPKYG6GZX87, BGR122339001000, TGR800433747</t>
+          <t>BGR122339001000, L2138006SQBPKYG6GZX87, TGR800433747</t>
         </is>
       </c>
       <c r="C23" s="13" t="n">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>TGR997521479, L213800TBZBVWRUAOPV78, BGR140330201000</t>
+          <t>L213800TBZBVWRUAOPV78, TGR997521479, BGR140330201000</t>
         </is>
       </c>
       <c r="C25" s="13" t="n">
@@ -1967,7 +1967,7 @@
       </c>
       <c r="B26" s="6" t="inlineStr">
         <is>
-          <t>BGR141064201000, L213800PZN3W777G7XR07, TGR800792234</t>
+          <t>TGR800792234, BGR141064201000, L213800PZN3W777G7XR07</t>
         </is>
       </c>
       <c r="C26" s="11" t="n">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>BGR142754460000, TGR997010182, L254900CCGB73PBHKXL72</t>
+          <t>L254900CCGB73PBHKXL72, BGR142754460000, TGR997010182</t>
         </is>
       </c>
       <c r="C27" s="13" t="n">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="B28" s="6" t="inlineStr">
         <is>
-          <t>L9845007DB3RB2B4DN624, TGR800903737, BGR144560003000</t>
+          <t>TGR800903737, BGR144560003000, L9845007DB3RB2B4DN624</t>
         </is>
       </c>
       <c r="C28" s="11" t="n">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>BGR144725001000, TGR800911079</t>
+          <t>TGR800911079, BGR144725001000</t>
         </is>
       </c>
       <c r="C29" s="13" t="n">
@@ -2087,7 +2087,7 @@
       </c>
       <c r="B30" s="6" t="inlineStr">
         <is>
-          <t>TGR801077433, BGR148547901000, L213800DTEZE6R8BZ9K19</t>
+          <t>L213800DTEZE6R8BZ9K19, BGR148547901000, TGR801077433</t>
         </is>
       </c>
       <c r="C30" s="11" t="n">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>L213800XKY8GHKN57D970, TGR996899546, BGR152321260000</t>
+          <t>BGR152321260000, L213800XKY8GHKN57D970, TGR996899546</t>
         </is>
       </c>
       <c r="C31" s="13" t="n">
@@ -2139,7 +2139,7 @@
       </c>
       <c r="B32" s="6" t="inlineStr">
         <is>
-          <t>BGR153787304000, L9845007855485B71CC46, TGR801296814</t>
+          <t>TGR801296814, BGR153787304000, L9845007855485B71CC46</t>
         </is>
       </c>
       <c r="C32" s="11" t="n">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>BGR154382104000, TGR801322351</t>
+          <t>TGR801322351, BGR154382104000</t>
         </is>
       </c>
       <c r="C33" s="13" t="n">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="B34" s="6" t="inlineStr">
         <is>
-          <t>TGR801446716, L9845003A111B06B9D568, BGR157033507000</t>
+          <t>L9845003A111B06B9D568, TGR801446716, BGR157033507000</t>
         </is>
       </c>
       <c r="C34" s="11" t="n">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>TGR801446949, BGR157036301000, L9845004F1F377E786787</t>
+          <t>TGR801446949, L9845004F1F377E786787, BGR157036301000</t>
         </is>
       </c>
       <c r="C35" s="13" t="n">
@@ -2259,7 +2259,7 @@
       </c>
       <c r="B36" s="6" t="inlineStr">
         <is>
-          <t>L2138006VXU6UDW7P6H67, TGR801470046, BGR157511601000</t>
+          <t>BGR157511601000, TGR801470046, L2138006VXU6UDW7P6H67</t>
         </is>
       </c>
       <c r="C36" s="11" t="n">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>TGR996764210, BGR157802360000</t>
+          <t>BGR157802360000, TGR996764210</t>
         </is>
       </c>
       <c r="C37" s="13" t="n">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="B38" s="6" t="inlineStr">
         <is>
-          <t>TGR801554045, L213800YJOZGHVAPEJP93, BGR159031301000</t>
+          <t>TGR801554045, BGR159031301000, L213800YJOZGHVAPEJP93</t>
         </is>
       </c>
       <c r="C38" s="11" t="n">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>BGR160110060000, L2138006STLTDFRIZTC42, TGR996805731</t>
+          <t>BGR160110060000, TGR996805731, L2138006STLTDFRIZTC42</t>
         </is>
       </c>
       <c r="C39" s="13" t="n">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="B40" s="6" t="inlineStr">
         <is>
-          <t>TGR801698110, L984500E6O0A11A6C4E59, BGR161709401000</t>
+          <t>L984500E6O0A11A6C4E59, TGR801698110, BGR161709401000</t>
         </is>
       </c>
       <c r="C40" s="11" t="n">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>BGR000861301000, L213800MU91F1752AVM79, TGR094321237</t>
+          <t>L213800MU91F1752AVM79, BGR000861301000, TGR094321237</t>
         </is>
       </c>
       <c r="C41" s="13" t="n">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>BGR165052501000, TGR801878297, L984500F87AF5652C5A91</t>
+          <t>L984500F87AF5652C5A91, BGR165052501000, TGR801878297</t>
         </is>
       </c>
       <c r="C43" s="13" t="n">
@@ -2491,8 +2491,8 @@
       </c>
       <c r="B44" s="6" t="inlineStr">
         <is>
-          <t>TGR802025852,  
-BGR168398401000, BGR168398401000</t>
+          <t xml:space="preserve"> 
+BGR168398401000, BGR168398401000, TGR802025852</t>
         </is>
       </c>
       <c r="C44" s="11" t="n">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>BGR168862301000, TGR802047322, L2138007QOK3W75DIHX50</t>
+          <t>TGR802047322, BGR168862301000, L2138007QOK3W75DIHX50</t>
         </is>
       </c>
       <c r="C45" s="13" t="n">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>BGR171519601000, TGR802177269, L984500EE58FDEBF8BF32</t>
+          <t>L984500EE58FDEBF8BF32, TGR802177269, BGR171519601000</t>
         </is>
       </c>
       <c r="C47" s="13" t="n">
@@ -2612,7 +2612,7 @@
       </c>
       <c r="B48" s="6" t="inlineStr">
         <is>
-          <t>TGR802187644, BGR171720006000</t>
+          <t>BGR171720006000, TGR802187644</t>
         </is>
       </c>
       <c r="C48" s="11" t="n">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>BGR171775701000, TGR802190685</t>
+          <t>TGR802190685, BGR171775701000</t>
         </is>
       </c>
       <c r="C49" s="13" t="n">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="B50" s="6" t="inlineStr">
         <is>
-          <t>L213800G7J7NDXVAS3P11, TGR996542649, BGR173975960000</t>
+          <t>L213800G7J7NDXVAS3P11, BGR173975960000, TGR996542649</t>
         </is>
       </c>
       <c r="C50" s="11" t="n">
@@ -2702,7 +2702,7 @@
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>BGR174106158000, TGR996723817</t>
+          <t>TGR996723817, BGR174106158000</t>
         </is>
       </c>
       <c r="C51" s="13" t="n">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B52" s="6" t="inlineStr">
         <is>
-          <t>TGR802458356, BGR176733801000</t>
+          <t>BGR176733801000, TGR802458356</t>
         </is>
       </c>
       <c r="C52" s="11" t="n">
@@ -5175,7 +5175,7 @@
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>BGR003882701000, TGR099759863, L213800USGL7Q5UR9M221</t>
+          <t>L213800USGL7Q5UR9M221, BGR003882701000, TGR099759863</t>
         </is>
       </c>
       <c r="C59" s="13" t="n">
@@ -5685,11 +5685,7 @@
           <t>EGRMFMC005</t>
         </is>
       </c>
-      <c r="H71" s="4" t="inlineStr">
-        <is>
-          <t>PEGRAK00809_SHR</t>
-        </is>
-      </c>
+      <c r="H71" s="4" t="inlineStr"/>
       <c r="I71" s="4" t="inlineStr"/>
     </row>
     <row r="72" ht="36" customHeight="1">
@@ -5700,7 +5696,7 @@
       </c>
       <c r="B72" s="6" t="inlineStr">
         <is>
-          <t>L213800U7SBKWW79CBG88, TGR099554901, BGR003548801000</t>
+          <t>L213800U7SBKWW79CBG88, BGR003548801000, TGR099554901</t>
         </is>
       </c>
       <c r="C72" s="11" t="n">
@@ -5882,11 +5878,7 @@
           <t>EGRMFMC005</t>
         </is>
       </c>
-      <c r="H76" s="6" t="inlineStr">
-        <is>
-          <t>PEGRAK00265_SHR</t>
-        </is>
-      </c>
+      <c r="H76" s="6" t="inlineStr"/>
       <c r="I76" s="6" t="inlineStr"/>
     </row>
     <row r="77" ht="36" customHeight="1">
@@ -7209,7 +7201,7 @@
       </c>
       <c r="B109" s="4" t="inlineStr">
         <is>
-          <t>BGR003546201000, TGR099555020, L549300XDXYOF57JOFT72</t>
+          <t>TGR099555020, BGR003546201000, L549300XDXYOF57JOFT72</t>
         </is>
       </c>
       <c r="C109" s="13" t="n">
@@ -7894,7 +7886,7 @@
       </c>
       <c r="B126" s="6" t="inlineStr">
         <is>
-          <t>L213800QM2ZFRARYU6C87, TGR800397001, BGR120108101000</t>
+          <t>TGR800397001, BGR120108101000, L213800QM2ZFRARYU6C87</t>
         </is>
       </c>
       <c r="C126" s="11" t="n">
@@ -8173,7 +8165,7 @@
       </c>
       <c r="B133" s="4" t="inlineStr">
         <is>
-          <t>L213800DDNBUCO6A2RT84, BGR131359701000, TGR800596087</t>
+          <t>TGR800596087, L213800DDNBUCO6A2RT84, BGR131359701000</t>
         </is>
       </c>
       <c r="C133" s="13" t="n">
@@ -8337,7 +8329,7 @@
       </c>
       <c r="B137" s="4" t="inlineStr">
         <is>
-          <t>TGR997521479, L213800TBZBVWRUAOPV78, BGR140330201000</t>
+          <t>L213800TBZBVWRUAOPV78, TGR997521479, BGR140330201000</t>
         </is>
       </c>
       <c r="C137" s="13" t="n">
@@ -8780,7 +8772,7 @@
       </c>
       <c r="B148" s="6" t="inlineStr">
         <is>
-          <t>TGR801077433, BGR148547901000, L213800DTEZE6R8BZ9K19</t>
+          <t>L213800DTEZE6R8BZ9K19, BGR148547901000, TGR801077433</t>
         </is>
       </c>
       <c r="C148" s="11" t="n">
@@ -8940,7 +8932,7 @@
       </c>
       <c r="B152" s="6" t="inlineStr">
         <is>
-          <t>L213800XKY8GHKN57D970, TGR996899546, BGR152321260000</t>
+          <t>BGR152321260000, L213800XKY8GHKN57D970, TGR996899546</t>
         </is>
       </c>
       <c r="C152" s="11" t="n">
@@ -9543,7 +9535,7 @@
       </c>
       <c r="B167" s="4" t="inlineStr">
         <is>
-          <t>BGR160110060000, L2138006STLTDFRIZTC42, TGR996805731</t>
+          <t>BGR160110060000, TGR996805731, L2138006STLTDFRIZTC42</t>
         </is>
       </c>
       <c r="C167" s="13" t="n">
@@ -9826,7 +9818,7 @@
       </c>
       <c r="B174" s="6" t="inlineStr">
         <is>
-          <t>BGR000861301000, L213800MU91F1752AVM79, TGR094321237</t>
+          <t>L213800MU91F1752AVM79, BGR000861301000, TGR094321237</t>
         </is>
       </c>
       <c r="C174" s="11" t="n">
@@ -11971,7 +11963,7 @@
       </c>
       <c r="B227" s="4" t="inlineStr">
         <is>
-          <t>BGR174106158000, TGR996723817</t>
+          <t>TGR996723817, BGR174106158000</t>
         </is>
       </c>
       <c r="C227" s="13" t="n">
@@ -12883,11 +12875,7 @@
           <t>EGR802458356</t>
         </is>
       </c>
-      <c r="H249" s="4" t="inlineStr">
-        <is>
-          <t>PEGRAK01102_SHR</t>
-        </is>
-      </c>
+      <c r="H249" s="4" t="inlineStr"/>
       <c r="I249" s="4" t="inlineStr"/>
     </row>
     <row r="250" ht="36" customHeight="1">
@@ -13140,7 +13128,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D341"/>
+  <dimension ref="A1:D339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -19638,7 +19626,7 @@
       <c r="C330" s="6" t="inlineStr"/>
       <c r="D330" s="6" t="inlineStr">
         <is>
-          <t>EGRAK01002, EGRAK01102</t>
+          <t>EGRAK01002</t>
         </is>
       </c>
     </row>
@@ -19808,36 +19796,8 @@
         </is>
       </c>
     </row>
-    <row r="340" ht="36" customHeight="1">
-      <c r="A340" s="10" t="inlineStr">
-        <is>
-          <t>PEGRAK00265_SHR</t>
-        </is>
-      </c>
-      <c r="B340" s="11" t="inlineStr"/>
-      <c r="C340" s="6" t="inlineStr"/>
-      <c r="D340" s="6" t="inlineStr">
-        <is>
-          <t>EGRAK00265</t>
-        </is>
-      </c>
-    </row>
-    <row r="341" ht="36" customHeight="1">
-      <c r="A341" s="12" t="inlineStr">
-        <is>
-          <t>PEGRAK00809_SHR</t>
-        </is>
-      </c>
-      <c r="B341" s="13" t="inlineStr"/>
-      <c r="C341" s="4" t="inlineStr"/>
-      <c r="D341" s="4" t="inlineStr">
-        <is>
-          <t>EGRAK00809</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D341"/>
+  <autoFilter ref="A1:D339"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>